<commit_message>
Documents: - Ajout d'une documentation propre avec Description du projet.docx - Ajout des illustrations dans Illustrations.pptx
Scilab:
- Correction filtrage à moyenne glissante dans Filtrage.sci
- Ajout d'une fonction pour reprendre l'horodatage d'un relevé avec Modifier_Horodatage.sci
- Intégration de cette fonction dans GESTION_RELEVES.sce
- Correction légende HP/HC dans Tracer_Graph.sci
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -177,6 +177,9 @@
   <si>
     <t>Date
 cloture</t>
+  </si>
+  <si>
+    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 20*fsignal = 24kHz)</t>
   </si>
 </sst>
 </file>
@@ -330,21 +333,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF93333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -668,10 +657,10 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -752,7 +741,7 @@
     <row r="2" spans="1:18" ht="15.75">
       <c r="C2" s="3">
         <f>COUNTIF(F5:F59,C1)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7">
         <f>COUNTIF(F5:F59,D1)</f>
@@ -764,11 +753,11 @@
       </c>
       <c r="F2" s="6">
         <f>MAX(A5:A59)+1</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="10">
         <f>COUNTIF(B5:B59,L1)+COUNTIF(B5:B59,M1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="6">
         <f>COUNTIF(D5:D59,"X")</f>
@@ -776,7 +765,7 @@
       </c>
       <c r="I2" s="6">
         <f>COUNTIF(E5:E59,"X")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>1</v>
@@ -1531,18 +1520,31 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="6" t="str">
-        <f>IF(B30&lt;&gt;"",MAX($A$5:A29)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="3"/>
+    <row r="30" spans="1:9" ht="30">
+      <c r="A30" s="6">
+        <v>25</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4">
+        <v>41874</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
@@ -1900,16 +1902,16 @@
     <sortCondition ref="B3:B20"/>
   </sortState>
   <conditionalFormatting sqref="G5:G26 G30:G37">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(F5=$D$1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G59">
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>IF(OR(B5=$L$1,B5=$M$1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Attention" error="Sélectionner une proposition" prompt="Type d'action" sqref="B5:B59">
       <formula1>$L$1:$R$1</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
MAJ: Gestion des tickets
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="52">
   <si>
     <t>Type</t>
   </si>
@@ -159,16 +159,6 @@
     <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation</t>
   </si>
   <si>
-    <t>Contraire le changement de jour pour garantir la cloture du fichier
-Envisager de tester 00:01:00 ?!</t>
-  </si>
-  <si>
-    <t>Enregistrer les index à +/- 1 seconde</t>
-  </si>
-  <si>
-    <t>Lors de l'enregistrement du courant max; veiller à ce qu'il n'ai pas déjà été remis à 0</t>
-  </si>
-  <si>
     <t>Récupérer le répertoire par ftp
 http://help.scilab.org/docs/5.5.0/en_US/getURL.html
 =&gt; ne permet pas le fonctionnement voulu; essayer avec un script windows (.bat), tester sur un serveur Fillezilla
@@ -179,7 +169,21 @@
 cloture</t>
   </si>
   <si>
-    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 20*fsignal = 24kHz)</t>
+    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 10*fsignal = 12kHz)</t>
+  </si>
+  <si>
+    <t>Remplacer le - de Papp dans HCHP par 0
+Retirer les lignes vides à la fin lors d'un relevé HCHP (dernière ligne + celle avant mot d'état/Imax)</t>
+  </si>
+  <si>
+    <t>Contraindre le changement de jour pour garantir la cloture du fichier
+Envisager de tester 00:01:00 ?!</t>
+  </si>
+  <si>
+    <t>Enregistrer les index à +/- 1 seconde de l'heure entière</t>
+  </si>
+  <si>
+    <t>Lors de l'enregistrement du courant max; veiller à ce qu'il n'est pas déjà été remis à 0</t>
   </si>
 </sst>
 </file>
@@ -657,10 +661,10 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -741,7 +745,7 @@
     <row r="2" spans="1:18" ht="15.75">
       <c r="C2" s="3">
         <f>COUNTIF(F5:F59,C1)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="7">
         <f>COUNTIF(F5:F59,D1)</f>
@@ -753,11 +757,11 @@
       </c>
       <c r="F2" s="6">
         <f>MAX(A5:A59)+1</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="10">
         <f>COUNTIF(B5:B59,L1)+COUNTIF(B5:B59,M1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6">
         <f>COUNTIF(D5:D59,"X")</f>
@@ -765,7 +769,7 @@
       </c>
       <c r="I2" s="6">
         <f>COUNTIF(E5:E59,"X")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>1</v>
@@ -824,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>3</v>
@@ -1378,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H24" s="4">
         <v>41768</v>
@@ -1459,7 +1463,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H27" s="12">
         <v>41782</v>
@@ -1486,7 +1490,7 @@
         <v>8</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H28" s="12">
         <v>41782</v>
@@ -1513,7 +1517,7 @@
         <v>8</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H29" s="12">
         <v>41782</v>
@@ -1540,25 +1544,38 @@
         <v>8</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H30" s="4">
         <v>41874</v>
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="6" t="str">
-        <f>IF(B31&lt;&gt;"",MAX($A$5:A30)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="3"/>
+    <row r="31" spans="1:9" ht="45">
+      <c r="A31" s="6">
+        <v>26</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="4">
+        <v>41883</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">

</xml_diff>

<commit_message>
MAJ du fichier de suivit
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Suivit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$I$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="57">
   <si>
     <t>Type</t>
   </si>
@@ -73,12 +73,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Configurer l'UART par le code</t>
-  </si>
-  <si>
-    <t>Problème de documentation avec Doxygen</t>
-  </si>
-  <si>
     <t>Utiliser l'algo de détection de rupture pour filtrer la Papp</t>
   </si>
   <si>
@@ -97,27 +91,15 @@
     <t>Interface Android</t>
   </si>
   <si>
-    <t>Diffuser le projet (dépôt sur GITHUB, …)</t>
-  </si>
-  <si>
     <t>LIVRAISON</t>
   </si>
   <si>
     <t>DOCUMENTATION</t>
   </si>
   <si>
-    <t>Documentation pour la configuration R-Pi</t>
-  </si>
-  <si>
-    <t>Documentation pour l'utilisation des scripts Scilab</t>
-  </si>
-  <si>
     <t>Documentation du code source R-Pi</t>
   </si>
   <si>
-    <t>Mise en œuvre de la génération automatique de schémas (www.graphviz.org)</t>
-  </si>
-  <si>
     <t>MINEUR</t>
   </si>
   <si>
@@ -127,27 +109,7 @@
     <t>SAUVEGARDE</t>
   </si>
   <si>
-    <t>Réaliser une image de la carte SD avec le pilote de la clef Wifi fonctionnel</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Ne pas afficher les secondes sur le graphique, seulement hh:mm</t>
-  </si>
-  <si>
-    <t>Modifier la méthode d'import des lignes txt (cf strsplit)</t>
-  </si>
-  <si>
-    <t>Modifier le séparateur '\t' par ';' dans les enregistrements txt (Scilab,  cf strsplit)</t>
-  </si>
-  <si>
-    <t>Graphs permettant de représenter une machine d'état
-http://www.stack.nl/~dimitri/doxygen/manual/diagrams.html</t>
-  </si>
-  <si>
-    <t>Documentation du code source Scilab
-Extension pour Mathlab : http://www.stack.nl/~dimitri/doxygen/helpers.html</t>
   </si>
   <si>
     <t>Getting WN725N V2 working as an access point
@@ -159,31 +121,258 @@
     <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation</t>
   </si>
   <si>
-    <t>Récupérer le répertoire par ftp
+    <t>Date
+cloture</t>
+  </si>
+  <si>
+    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 10*fsignal = 12kHz)</t>
+  </si>
+  <si>
+    <t>Contraindre le changement de jour pour garantir la cloture du fichier
+Envisager de tester 00:01:00 ?!</t>
+  </si>
+  <si>
+    <t>Enregistrer les index à +/- 1 seconde de l'heure entière</t>
+  </si>
+  <si>
+    <t>Lors de l'enregistrement du courant max; veiller à ce qu'il n'est pas déjà été remis à 0</t>
+  </si>
+  <si>
+    <t>Gérérer "manuellement" la documentation Scilab, cf mail + #04, 13 et 15</t>
+  </si>
+  <si>
+    <r>
+      <t>Modifier le séparateur '\t' par ';' dans les enregistrements txt (Scilab,  cf strsplit)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; OK paramètre recherché passé par variable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Diffuser le projet (dépôt sur GITHUB, …)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; OK https://github.com/sebastien0/RPi.SuivitTRElec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Documentation pour l'utilisation des scripts Scilab</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; NOK, traité "manuellement", cf #27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documentation du code source Scilab
+Extension pour Mathlab : http://www.stack.nl/~dimitri/doxygen/helpers.html </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; NOK, traité "manuellement", cf #27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Modifier la méthode d'import des lignes txt (cf strsplit)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; OK, gain de temps environ 1:2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problème de documentation avec Doxygen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; NOK, traité "manuellement", cf #27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ne pas afficher les secondes sur le graphique, seulement hh:mm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; OK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documentation pour la configuration R-Pi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; 22/09/2014: Documentation projet OK, RAF: configuration R-Pi + interface (contenu des fichiers CSV)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Réaliser une image de la carte SD avec le pilote de la clef Wifi fonctionnel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; 22/09/2014: Image de sauvegarde réalisée, en refaire une plus propre serait mieux</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mise en œuvre de la génération automatique de schémas (www.graphviz.org) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; Redondant avec #20, clos</t>
+    </r>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Graphs permettant de représenter une machine d'état
+http://www.stack.nl/~dimitri/doxygen/manual/diagrams.html
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; 22/09/2014: Algo représentés dans la doc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Configurer l'UART par le code </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; 11/11/2013: Code\test\uart.c</t>
+    </r>
+  </si>
+  <si>
+    <t>Forcer la mise à jour de l'heure réguliairement (client NTP =&gt; ntpdate https://wiki.debian.org/fr/NTP)</t>
+  </si>
+  <si>
+    <t>Protéger par mot de passe toutes les connexions (accès web compris)!
+Crypter le contenu de la SD?</t>
+  </si>
+  <si>
+    <r>
+      <t>Récupérer le répertoire par ftp
 http://help.scilab.org/docs/5.5.0/en_US/getURL.html
 =&gt; ne permet pas le fonctionnement voulu; essayer avec un script windows (.bat), tester sur un serveur Fillezilla
-08/06/2014 Ok vers server Seb_Bureau =&gt; Essayer script vers R-Pi</t>
-  </si>
-  <si>
-    <t>Date
-cloture</t>
-  </si>
-  <si>
-    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 10*fsignal = 12kHz)</t>
+08/06/2014 Ok vers server Seb_Bureau</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; 22/09/2014: NOK vers R-Pi, protocole SFTP, non géré par Win =&gt; Ne sera jamais traité, utilisation manuelle de FileZilla</t>
+    </r>
   </si>
   <si>
     <t>Remplacer le - de Papp dans HCHP par 0
-Retirer les lignes vides à la fin lors d'un relevé HCHP (dernière ligne + celle avant mot d'état/Imax)</t>
-  </si>
-  <si>
-    <t>Contraindre le changement de jour pour garantir la cloture du fichier
-Envisager de tester 00:01:00 ?!</t>
-  </si>
-  <si>
-    <t>Enregistrer les index à +/- 1 seconde de l'heure entière</t>
-  </si>
-  <si>
-    <t>Lors de l'enregistrement du courant max; veiller à ce qu'il n'est pas déjà été remis à 0</t>
+Retirer les lignes vides à la fin lors d'un relevé HCHP (dernière ligne + celle avant mot d'état/Imax)
+Ajouter le type de constrat souscrit
+A faire aussi sur les relevés déjà obtenus</t>
+  </si>
+  <si>
+    <t>Générer la documentation dans un format HTML.
+Modifier le contenu de fichiers doxygen ?!</t>
   </si>
 </sst>
 </file>
@@ -193,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +393,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -341,14 +538,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF93333"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFF93333"/>
         </patternFill>
       </fill>
     </dxf>
@@ -658,13 +855,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -673,138 +870,138 @@
     <col min="2" max="2" width="17.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="66.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="13.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="2"/>
+    <col min="5" max="6" width="11.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="69" style="2" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75">
-      <c r="C1" s="5" t="str">
-        <f>L4</f>
+    <row r="1" spans="1:19" ht="15.75">
+      <c r="D1" s="5" t="str">
+        <f>M4</f>
         <v>Ouvert</v>
       </c>
-      <c r="D1" s="9" t="str">
-        <f>M4</f>
+      <c r="E1" s="9" t="str">
+        <f>N4</f>
         <v>En cours</v>
       </c>
-      <c r="E1" s="5" t="str">
-        <f>N4</f>
+      <c r="F1" s="5" t="str">
+        <f>O4</f>
         <v>Clos</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="9" t="str">
-        <f>CONCATENATE("dont ",L1," ou ",M1)</f>
+      <c r="G1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="9" t="str">
+        <f>CONCATENATE("dont ",M1," ou ",N1)</f>
         <v>dont BUG ou CORRECTION</v>
       </c>
-      <c r="H1" s="9" t="str">
+      <c r="I1" s="9" t="str">
         <f>CONCATENATE("Total ",D4)</f>
         <v>Total Scilab</v>
       </c>
-      <c r="I1" s="9" t="str">
+      <c r="J1" s="9" t="str">
         <f>CONCATENATE("Total ",E4)</f>
         <v>Total R-Pi</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="P1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75">
+      <c r="D2" s="3">
+        <f>COUNTIF(G5:G59,D1)</f>
+        <v>14</v>
+      </c>
+      <c r="E2" s="7">
+        <f>COUNTIF(G5:G59,E1)</f>
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <f>COUNTIF(G5:G59,F1)</f>
+        <v>10</v>
+      </c>
+      <c r="G2" s="6">
+        <f>MAX(A5:A59)+1</f>
+        <v>31</v>
+      </c>
+      <c r="H2" s="10">
+        <f>COUNTIF(B5:B59,M1)+COUNTIF(B5:B59,N1)</f>
+        <v>9</v>
+      </c>
+      <c r="I2" s="6">
+        <f>COUNTIF(D5:D59,"X")</f>
+        <v>14</v>
+      </c>
+      <c r="J2" s="6">
+        <f>COUNTIF(E5:E59,"X")</f>
+        <v>20</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75">
-      <c r="C2" s="3">
-        <f>COUNTIF(F5:F59,C1)</f>
-        <v>17</v>
-      </c>
-      <c r="D2" s="7">
-        <f>COUNTIF(F5:F59,D1)</f>
-        <v>8</v>
-      </c>
-      <c r="E2" s="3">
-        <f>COUNTIF(F5:F59,E1)</f>
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <f>MAX(A5:A59)+1</f>
-        <v>27</v>
-      </c>
-      <c r="G2" s="10">
-        <f>COUNTIF(B5:B59,L1)+COUNTIF(B5:B59,M1)</f>
-        <v>8</v>
-      </c>
-      <c r="H2" s="6">
-        <f>COUNTIF(D5:D59,"X")</f>
-        <v>12</v>
-      </c>
-      <c r="I2" s="6">
-        <f>COUNTIF(E5:E59,"X")</f>
-        <v>18</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75">
-      <c r="K3" s="16" t="s">
+      <c r="R2" s="11"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="L3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="M3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="33" customHeight="1">
+      <c r="R3" s="11"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="33" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>0</v>
@@ -818,36 +1015,39 @@
       <c r="E4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="16" t="s">
+      <c r="J4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" hidden="1">
+      <c r="R4" s="11"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" hidden="1">
       <c r="A5" s="6">
         <v>0</v>
       </c>
@@ -864,19 +1064,22 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>41765</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>41766</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30">
+    <row r="6" spans="1:19" ht="30" hidden="1">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -893,17 +1096,22 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="4">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="4">
         <v>41766</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="J6" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -920,76 +1128,85 @@
         <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="H7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="4">
         <v>41334</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="4">
+        <v>41766</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="H9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="4">
         <v>41766</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="4">
-        <v>41766</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="30" hidden="1">
       <c r="A10" s="6">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -1001,22 +1218,27 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="4">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4">
         <v>41766</v>
       </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" ht="45">
+      <c r="J10" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -1028,22 +1250,25 @@
         <v>16</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="H11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="4">
         <v>41766</v>
       </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>7</v>
@@ -1055,22 +1280,25 @@
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="H12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="4">
         <v>41766</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" ht="30" hidden="1">
       <c r="A13" s="6">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -1082,49 +1310,57 @@
         <v>17</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="4">
+        <v>41766</v>
+      </c>
+      <c r="J13" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="6">
         <v>9</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="4">
         <v>41766</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="6">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="4">
-        <v>41766</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" ht="45">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" ht="60" hidden="1">
       <c r="A15" s="6">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
@@ -1136,42 +1372,52 @@
         <v>17</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>41766</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" ht="30">
+      <c r="J15" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="45">
       <c r="A16" s="6">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="H16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="4">
         <v>41766</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" hidden="1">
       <c r="A17" s="6">
         <v>2</v>
       </c>
@@ -1179,7 +1425,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -1188,17 +1434,22 @@
         <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="4">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="4">
         <v>41766</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" hidden="1">
       <c r="A18" s="6">
         <v>4</v>
       </c>
@@ -1206,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -1215,125 +1466,142 @@
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="4">
+        <v>41766</v>
+      </c>
+      <c r="J18" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" s="6">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="H19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="4">
         <v>41766</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="6">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6">
+        <v>14</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="H20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="4">
         <v>41766</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="6">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="4">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" hidden="1">
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4">
         <v>41766</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="6">
+      <c r="J21" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45">
+      <c r="A22" s="6">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="4">
+      <c r="H22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="4">
         <v>41766</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="30">
-      <c r="A22" s="6">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="4">
-        <v>41766</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" hidden="1">
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="6">
         <v>18</v>
       </c>
@@ -1341,7 +1609,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
@@ -1350,27 +1618,30 @@
         <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="4">
-        <v>41768</v>
+      <c r="H23" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="I23" s="4">
         <v>41768</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="75">
+      <c r="J23" s="4">
+        <v>41768</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="105">
       <c r="A24" s="6">
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
@@ -1379,25 +1650,30 @@
         <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="4">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="4">
         <v>41768</v>
       </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="30">
+      <c r="J24" s="4">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="6">
         <v>20</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>16</v>
@@ -1406,25 +1682,28 @@
         <v>16</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="4">
+        <v>17</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="4">
         <v>41768</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="60">
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="60">
       <c r="A26" s="6">
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>17</v>
@@ -1433,17 +1712,20 @@
         <v>16</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="H26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="4">
         <v>41768</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="30">
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" ht="30">
       <c r="A27" s="3">
         <v>22</v>
       </c>
@@ -1460,17 +1742,20 @@
         <v>16</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="12">
+      <c r="H27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="4">
         <v>41782</v>
       </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="3">
         <v>23</v>
       </c>
@@ -1478,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>17</v>
@@ -1487,17 +1772,20 @@
         <v>16</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="12">
+      <c r="H28" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="12">
         <v>41782</v>
       </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" ht="30">
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="3">
         <v>24</v>
       </c>
@@ -1505,7 +1793,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>17</v>
@@ -1514,17 +1802,20 @@
         <v>16</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="12">
+      <c r="H29" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="12">
         <v>41782</v>
       </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" ht="30">
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" ht="30">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1541,17 +1832,20 @@
         <v>16</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="4">
+      <c r="H30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="4">
         <v>41874</v>
       </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="45">
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" ht="75">
       <c r="A31" s="6">
         <v>26</v>
       </c>
@@ -1562,351 +1856,437 @@
         <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="H31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="4">
         <v>41883</v>
       </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="6" t="str">
-        <f>IF(B32&lt;&gt;"",MAX($A$5:A31)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="6" t="str">
-        <f>IF(B33&lt;&gt;"",MAX($A$5:A32)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="6" t="str">
-        <f>IF(B34&lt;&gt;"",MAX($A$5:A33)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="6" t="str">
-        <f>IF(B35&lt;&gt;"",MAX($A$5:A34)+1,"")</f>
-        <v/>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="6" t="str">
-        <f>IF(B36&lt;&gt;"",MAX($A$5:A35)+1,"")</f>
-        <v/>
-      </c>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="6">
+        <v>27</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="4">
+        <v>41904</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" ht="30">
+      <c r="A33" s="6">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="4">
+        <v>41906</v>
+      </c>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" ht="30">
+      <c r="A34" s="6">
+        <v>29</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" s="4">
+        <v>41916</v>
+      </c>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" ht="30">
+      <c r="A35" s="6">
+        <v>30</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="4">
+        <v>41917</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="6"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="6" t="str">
-        <f>IF(B37&lt;&gt;"",MAX($A$5:A36)+1,"")</f>
-        <v/>
-      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="6"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="11"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="11"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="11"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="11"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="11"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="13"/>
       <c r="I40" s="11"/>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="11"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="11"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="11"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="11"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="11"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="11"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="11"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="11"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="11"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="11"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="11"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="11"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="11"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="13"/>
       <c r="I47" s="11"/>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="11"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="11"/>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="11"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="13"/>
       <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="11"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="13"/>
       <c r="I50" s="11"/>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="11"/>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="11"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="13"/>
       <c r="I51" s="11"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="11"/>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="11"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="13"/>
       <c r="I52" s="11"/>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="11"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="13"/>
       <c r="I53" s="11"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="11"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="11"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="13"/>
       <c r="I54" s="11"/>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="11"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="13"/>
       <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="11"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="13"/>
       <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="11"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="13"/>
       <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="11"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="13"/>
       <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="11"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="13"/>
       <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:I36">
-    <filterColumn colId="5">
+  <autoFilter ref="A4:J37">
+    <filterColumn colId="5"/>
+    <filterColumn colId="6">
       <filters blank="1">
         <filter val="En cours"/>
         <filter val="Ouvert"/>
@@ -1918,28 +2298,28 @@
     <sortCondition ref="D3:D20"/>
     <sortCondition ref="B3:B20"/>
   </sortState>
-  <conditionalFormatting sqref="G5:G26 G30:G37">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF(F5=$D$1,1,0)</formula>
+  <conditionalFormatting sqref="H5:H59">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>IF(AND(OR(B5=$M$1,B5=$N$1),G5&lt;&gt;$O$4),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G59">
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>IF(OR(B5=$L$1,B5=$M$1),1,0)</formula>
+  <conditionalFormatting sqref="H5:H26 H30:H37">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>IF(G5=$E$1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Attention" error="Sélectionner une proposition" prompt="Type d'action" sqref="B5:B59">
-      <formula1>$L$1:$R$1</formula1>
+      <formula1>$M$1:$S$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Priorité" sqref="C5:C59">
-      <formula1>$L$2:$M$2</formula1>
+      <formula1>$M$2:$N$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Implantation" sqref="D5:E59">
-      <formula1>$L$3:$M$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Implantation" sqref="D5:F59">
+      <formula1>$M$3:$N$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Statut" sqref="F5:F59">
-      <formula1>$L$4:$N$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Statut" sqref="G5:G59">
+      <formula1>$M$4:$O$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1958,7 +2338,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G5:G33</xm:sqref>
+          <xm:sqref>H5:H33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1980,7 +2360,7 @@
           <x14:formula1>
             <xm:f>#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F33</xm:sqref>
+          <xm:sqref>G5:G33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Attention" error="Sélectionner une proposition" promptTitle="Implantation">
           <x14:formula1>

</xml_diff>

<commit_message>
Continuation intégration structure stcReleve
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -858,7 +858,7 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
@@ -946,11 +946,11 @@
       </c>
       <c r="E2" s="7">
         <f>COUNTIF(G5:G59,E1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3">
         <f>COUNTIF(G5:G59,F1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="6">
         <f>MAX(A5:A59)+1</f>
@@ -1633,7 +1633,7 @@
         <v>41768</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="105">
+    <row r="24" spans="1:10" ht="105" hidden="1">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
MAJ de l'arborescence /Documents: - Ajout d'un document d'installation et configuration du PC et R-Pi - Suppression drivers ou documents obsolètes
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Utiliser l'algo de détection de rupture pour filtrer la Papp</t>
   </si>
   <si>
     <t>Evolution</t>
@@ -123,9 +120,6 @@
   <si>
     <t>Date
 cloture</t>
-  </si>
-  <si>
-    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto. Simu à faire sous PSIM (fc &gt; 10*fsignal = 12kHz)</t>
   </si>
   <si>
     <t>Contraindre le changement de jour pour garantir la cloture du fichier
@@ -255,38 +249,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Documentation pour la configuration R-Pi </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=&gt; 22/09/2014: Documentation projet OK, RAF: configuration R-Pi + interface (contenu des fichiers CSV)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Réaliser une image de la carte SD avec le pilote de la clef Wifi fonctionnel </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=&gt; 22/09/2014: Image de sauvegarde réalisée, en refaire une plus propre serait mieux</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Mise en œuvre de la génération automatique de schémas (www.graphviz.org) </t>
     </r>
     <r>
@@ -306,24 +268,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Graphs permettant de représenter une machine d'état
-http://www.stack.nl/~dimitri/doxygen/manual/diagrams.html
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=&gt; 22/09/2014: Algo représentés dans la doc</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Configurer l'UART par le code </t>
     </r>
     <r>
@@ -373,6 +317,106 @@
   <si>
     <t>Générer la documentation dans un format HTML.
 Modifier le contenu de fichiers doxygen ?!</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Créer le wiki sur https://github.com/sebastien0/ConsoCompteurElectrique_avec_RPi/wiki</t>
+  </si>
+  <si>
+    <t>Graphs permettant de représenter une machine d'état
+http://www.stack.nl/~dimitri/doxygen/manual/diagrams.html
+=&gt; 22/09/2014: Algo représentés dans la doc
+11/01/2015 Génération automatique des graphs appelants et appelés</t>
+  </si>
+  <si>
+    <t>Utiliser l'algo de détection de rupture pour filtrer la Papp
+01/11/2014 Utilisation GlrBrandtMoy, paramètres à ajuster selon profil</t>
+  </si>
+  <si>
+    <r>
+      <t>Documentation pour la configuration R-Pi
+22/09/2014: Documentation projet OK, RAF: configuration R-Pi + interface (contenu des fichiers CSV)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+11/01/2015 Documentation en cours (Configurartion de la R-Pi.docx)</t>
+    </r>
+  </si>
+  <si>
+    <t>HARDWARE - Filtrer le signal provenant du compteur, en aval de l'opto avec une capa ou en amont avec une inductance de mode commun</t>
+  </si>
+  <si>
+    <t>Le programme peut enregistrer dans un log les premières trames reçues</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Réaliser une image de la carte SD avec le pilote de la clef Wifi fonctionnel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>22/09/2014: Image de sauvegarde réalisée, en refaire une plus propre serait mieux</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11/01/2015 Installation propre. Sauvegarde à faire lorsque débranché</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+27/04/2015 Sauvegarde réalisée</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -479,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -529,6 +573,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,10 +905,10 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -900,7 +947,7 @@
         <v>Clos</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="9" t="str">
         <f>CONCATENATE("dont ",M1," ou ",N1)</f>
@@ -927,34 +974,34 @@
         <v>5</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75">
       <c r="D2" s="3">
         <f>COUNTIF(G5:G59,D1)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7">
         <f>COUNTIF(G5:G59,E1)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3">
         <f>COUNTIF(G5:G59,F1)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G2" s="6">
         <f>MAX(A5:A59)+1</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H2" s="10">
         <f>COUNTIF(B5:B59,M1)+COUNTIF(B5:B59,N1)</f>
@@ -966,7 +1013,7 @@
       </c>
       <c r="J2" s="6">
         <f>COUNTIF(E5:E59,"X")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>1</v>
@@ -975,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -1001,7 +1048,7 @@
     </row>
     <row r="4" spans="1:19" ht="33" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>0</v>
@@ -1016,7 +1063,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>3</v>
@@ -1028,7 +1075,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>3</v>
@@ -1102,7 +1149,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I6" s="4">
         <v>41766</v>
@@ -1134,14 +1181,14 @@
         <v>9</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I7" s="4">
         <v>41334</v>
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" ht="30" hidden="1">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -1149,7 +1196,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -1161,25 +1208,27 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="I8" s="4">
         <v>41766</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="4">
+        <v>42015</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
@@ -1194,7 +1243,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="4">
         <v>41766</v>
@@ -1206,7 +1255,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -1224,7 +1273,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" s="4">
         <v>41766</v>
@@ -1256,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I11" s="4">
         <v>41766</v>
@@ -1286,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I12" s="4">
         <v>41766</v>
@@ -1298,7 +1347,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -1316,7 +1365,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I13" s="4">
         <v>41766</v>
@@ -1330,10 +1379,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>17</v>
@@ -1348,7 +1397,7 @@
         <v>8</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="4">
         <v>41766</v>
@@ -1360,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
@@ -1378,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I15" s="4">
         <v>41766</v>
@@ -1410,7 +1459,7 @@
         <v>8</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" s="4">
         <v>41766</v>
@@ -1425,7 +1474,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -1440,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I17" s="4">
         <v>41766</v>
@@ -1457,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -1472,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I18" s="4">
         <v>41766</v>
@@ -1481,12 +1530,12 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30">
+    <row r="19" spans="1:10" ht="60">
       <c r="A19" s="6">
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>7</v>
@@ -1504,7 +1553,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="I19" s="4">
         <v>41766</v>
@@ -1516,7 +1565,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>7</v>
@@ -1534,7 +1583,7 @@
         <v>9</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="4">
         <v>41766</v>
@@ -1546,10 +1595,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>17</v>
@@ -1564,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I21" s="4">
         <v>41766</v>
@@ -1573,12 +1622,12 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="45">
+    <row r="22" spans="1:10" ht="75" hidden="1">
       <c r="A22" s="6">
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>7</v>
@@ -1591,15 +1640,17 @@
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I22" s="4">
         <v>41766</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="J22" s="4">
+        <v>42121</v>
+      </c>
     </row>
     <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="6">
@@ -1609,7 +1660,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
@@ -1624,7 +1675,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I23" s="4">
         <v>41768</v>
@@ -1638,10 +1689,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
@@ -1656,7 +1707,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I24" s="4">
         <v>41768</v>
@@ -1665,15 +1716,15 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45">
+    <row r="25" spans="1:10" ht="60" hidden="1">
       <c r="A25" s="6">
         <v>20</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>17</v>
@@ -1685,25 +1736,27 @@
         <v>17</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="I25" s="4">
         <v>41768</v>
       </c>
-      <c r="J25" s="3"/>
+      <c r="J25" s="4">
+        <v>42015</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="60">
       <c r="A26" s="6">
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>17</v>
@@ -1718,7 +1771,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I26" s="4">
         <v>41768</v>
@@ -1748,7 +1801,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I27" s="4">
         <v>41782</v>
@@ -1763,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>17</v>
@@ -1778,7 +1831,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I28" s="12">
         <v>41782</v>
@@ -1793,7 +1846,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>17</v>
@@ -1808,7 +1861,7 @@
         <v>8</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I29" s="12">
         <v>41782</v>
@@ -1838,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="I30" s="4">
         <v>41874</v>
@@ -1868,7 +1921,7 @@
         <v>8</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I31" s="4">
         <v>41883</v>
@@ -1883,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -1898,7 +1951,7 @@
         <v>10</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I32" s="4">
         <v>41904</v>
@@ -1928,7 +1981,7 @@
         <v>8</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I33" s="4">
         <v>41906</v>
@@ -1958,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I34" s="4">
         <v>41916</v>
@@ -1970,10 +2023,10 @@
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>16</v>
@@ -1988,35 +2041,71 @@
         <v>8</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I35" s="4">
         <v>41917</v>
       </c>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="6"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="3"/>
+    <row r="36" spans="1:10" ht="30">
+      <c r="A36" s="6">
+        <v>31</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="4">
+        <v>42015</v>
+      </c>
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="6"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="3"/>
+      <c r="A37" s="6">
+        <v>32</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I37" s="4">
+        <v>42121</v>
+      </c>
       <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:10">
@@ -2287,7 +2376,7 @@
   <autoFilter ref="A4:J37">
     <filterColumn colId="5"/>
     <filterColumn colId="6">
-      <filters blank="1">
+      <filters>
         <filter val="En cours"/>
         <filter val="Ouvert"/>
       </filters>

</xml_diff>

<commit_message>
Mise à jour d'illustrations Reprise du projet et isolation de l'erreur "segfault"
</commit_message>
<xml_diff>
--- a/RaF R-Pi.xlsx
+++ b/RaF R-Pi.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Suivit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Suivit!$A$4:$J$38</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="62">
   <si>
     <t>Type</t>
   </si>
@@ -86,9 +86,6 @@
 http://raspberry-at-home.com/hotspot-wifi-access-point/
 En cas de problème :
 http://www.raspberrypi.org/forums/viewtopic.php?f=26&amp;t=49355</t>
-  </si>
-  <si>
-    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation</t>
   </si>
   <si>
     <t>Date
@@ -310,6 +307,17 @@
   <si>
     <t>Générer la Documentation dans un format HTML.
 Modifier le contenu de fichiers doxygen ?!</t>
+  </si>
+  <si>
+    <t>Calculer le cout d'une journée
+PHT/kWh = 0.0892€  - Base, règlementé, 6kVA</t>
+  </si>
+  <si>
+    <t>Instabilité du programme (Claix), utiliser Valgrind ou http://www.commentcamarche.net/faq/4791-langage-c-c-c-erreur-de-segmentation
+=&gt; Erreur isolée, se produit lorsque ETX est avant STX</t>
+  </si>
+  <si>
+    <t>Rejeté</t>
   </si>
 </sst>
 </file>
@@ -810,7 +818,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -867,35 +875,35 @@
         <v>0</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="S1" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="30">
       <c r="D2" s="15">
         <f>COUNTIF(G5:G59,D1)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="16">
         <f>COUNTIF(G5:G59,E1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="15">
         <f>COUNTIF(G5:G59,F1)</f>
@@ -911,7 +919,7 @@
       </c>
       <c r="I2" s="17">
         <f>COUNTIF(D5:D59,"X")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="17">
         <f>COUNTIF(E5:E59,"X")</f>
@@ -921,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -965,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>3</v>
@@ -977,7 +985,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>3</v>
@@ -991,20 +999,22 @@
       <c r="O4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="45">
+    <row r="5" spans="1:19" ht="60">
       <c r="A5" s="17">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>13</v>
@@ -1016,10 +1026,10 @@
         <v>13</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="I5" s="19">
         <v>41766</v>
@@ -1031,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -1049,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="3">
         <v>41766</v>
@@ -1063,10 +1073,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>13</v>
@@ -1081,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="19">
         <v>41334</v>
@@ -1093,10 +1103,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>13</v>
@@ -1111,22 +1121,22 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="19">
         <v>41782</v>
       </c>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="30" hidden="1">
       <c r="A9" s="17">
         <v>25</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>13</v>
@@ -1138,25 +1148,27 @@
         <v>13</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="19">
         <v>41874</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="19">
+        <v>43412</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="75">
       <c r="A10" s="17">
         <v>26</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>12</v>
@@ -1171,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="19">
         <v>41883</v>
@@ -1183,10 +1195,10 @@
         <v>28</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>13</v>
@@ -1201,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="19">
         <v>41906</v>
@@ -1213,10 +1225,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>13</v>
@@ -1231,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="20">
         <v>41782</v>
@@ -1243,10 +1255,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>13</v>
@@ -1261,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="20">
         <v>41782</v>
@@ -1273,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -1305,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1323,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="3">
         <v>41766</v>
@@ -1337,10 +1349,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>13</v>
@@ -1367,10 +1379,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>13</v>
@@ -1397,10 +1409,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>13</v>
@@ -1415,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="19">
         <v>41916</v>
@@ -1427,10 +1439,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>13</v>
@@ -1445,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I19" s="19">
         <v>42121</v>
@@ -1457,10 +1469,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1475,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="3">
         <v>41766</v>
@@ -1489,10 +1501,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
@@ -1507,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I21" s="3">
         <v>41766</v>
@@ -1521,10 +1533,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1539,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" s="3">
         <v>41768</v>
@@ -1553,10 +1565,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1571,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="3">
         <v>41904</v>
@@ -1583,10 +1595,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1601,7 +1613,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3">
         <v>41768</v>
@@ -1610,15 +1622,15 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="17">
-        <v>6</v>
+    <row r="25" spans="1:10" ht="30">
+      <c r="A25" s="15">
+        <v>31</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>12</v>
@@ -1632,29 +1644,29 @@
       <c r="G25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="19">
-        <v>41766</v>
-      </c>
-      <c r="J25" s="15"/>
+      <c r="H25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="20">
+        <v>42699</v>
+      </c>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>13</v>
@@ -1663,22 +1675,22 @@
         <v>4</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I26" s="19">
         <v>41766</v>
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="60">
+    <row r="27" spans="1:10">
       <c r="A27" s="17">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>13</v>
@@ -1693,10 +1705,10 @@
         <v>4</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I27" s="19">
-        <v>41768</v>
+        <v>41766</v>
       </c>
       <c r="J27" s="15"/>
     </row>
@@ -1705,10 +1717,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
@@ -1723,7 +1735,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I28" s="3">
         <v>41766</v>
@@ -1737,10 +1749,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>12</v>
@@ -1755,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I29" s="3">
         <v>41766</v>
@@ -1769,10 +1781,10 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>12</v>
@@ -1787,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I30" s="3">
         <v>41766</v>
@@ -1796,12 +1808,12 @@
         <v>41904</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30">
+    <row r="31" spans="1:10" ht="60">
       <c r="A31" s="17">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>55</v>
@@ -1810,61 +1822,61 @@
         <v>13</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="I31" s="19">
+        <v>41768</v>
+      </c>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:10" ht="30">
+      <c r="A32" s="17">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="19">
         <v>42015</v>
       </c>
-      <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:10" ht="60">
-      <c r="A32" s="17">
-        <v>12</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" s="19">
-        <v>41766</v>
-      </c>
       <c r="J32" s="15"/>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:10" ht="60">
       <c r="A33" s="17">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>13</v>
@@ -1879,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="I33" s="19">
         <v>41766</v>
@@ -1891,10 +1903,10 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>13</v>
@@ -1909,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I34" s="3">
         <v>41766</v>
@@ -1923,10 +1935,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>13</v>
@@ -1941,7 +1953,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I35" s="3">
         <v>41768</v>
@@ -1952,31 +1964,31 @@
     </row>
     <row r="36" spans="1:10" ht="30">
       <c r="A36" s="17">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="I36" s="19">
-        <v>41917</v>
+        <v>41766</v>
       </c>
       <c r="J36" s="15"/>
     </row>
@@ -1985,10 +1997,10 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -2001,7 +2013,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I37" s="3">
         <v>41766</v>
@@ -2010,17 +2022,35 @@
         <v>42121</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+    <row r="38" spans="1:10" ht="30">
+      <c r="A38" s="17">
+        <v>30</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="19">
+        <v>41917</v>
+      </c>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="15"/>
@@ -2275,7 +2305,7 @@
       <c r="J59" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J37">
+  <autoFilter ref="A4:J38">
     <filterColumn colId="5"/>
     <filterColumn colId="6">
       <filters>
@@ -2283,10 +2313,6 @@
         <filter val="Ouvert"/>
       </filters>
     </filterColumn>
-    <sortState ref="A5:J37">
-      <sortCondition ref="B5:B37"/>
-      <sortCondition ref="C5:C37"/>
-    </sortState>
   </autoFilter>
   <sortState ref="A3:I20">
     <sortCondition ref="E3:E20"/>
@@ -2314,7 +2340,7 @@
       <formula1>$M$3:$N$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Statut" sqref="G5:G59">
-      <formula1>$M$4:$O$4</formula1>
+      <formula1>$M$4:$P$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>